<commit_message>
initial tests working and successful.
</commit_message>
<xml_diff>
--- a/Our_ClueLayout.xlsx
+++ b/Our_ClueLayout.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\adit\Downloads\Clue game\Clue game\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8070"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24960" windowHeight="8070"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,9 +53,6 @@
     <t>O</t>
   </si>
   <si>
-    <t>w</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -93,6 +90,9 @@
   </si>
   <si>
     <t>LR</t>
+  </si>
+  <si>
+    <t>W</t>
   </si>
 </sst>
 </file>
@@ -441,7 +441,7 @@
   <dimension ref="A1:X27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y21" sqref="Y21"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,10 +457,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
@@ -469,40 +469,40 @@
         <v>0</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>4</v>
@@ -531,10 +531,10 @@
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>0</v>
@@ -543,40 +543,40 @@
         <v>0</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>4</v>
@@ -605,52 +605,52 @@
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>4</v>
@@ -679,10 +679,10 @@
         <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>0</v>
@@ -691,40 +691,40 @@
         <v>0</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>4</v>
@@ -747,16 +747,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>0</v>
@@ -765,49 +765,49 @@
         <v>0</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="U5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="W5" s="1" t="s">
         <v>4</v>
@@ -818,19 +818,19 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>0</v>
@@ -839,52 +839,52 @@
         <v>0</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="V6" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="W6" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="X6">
         <v>5</v>
@@ -892,73 +892,73 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="V7" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="X7">
         <v>6</v>
@@ -966,25 +966,25 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>1</v>
@@ -1017,22 +1017,22 @@
         <v>1</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="U8" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="V8" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="W8" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="X8">
         <v>7</v>
@@ -1040,25 +1040,25 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>1</v>
@@ -1091,22 +1091,22 @@
         <v>1</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="U9" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="V9" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="X9">
         <v>8</v>
@@ -1126,13 +1126,13 @@
         <v>7</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>1</v>
@@ -1165,19 +1165,19 @@
         <v>1</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="U10" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="V10" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="W10" s="1" t="s">
         <v>5</v>
@@ -1191,7 +1191,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>7</v>
@@ -1203,10 +1203,10 @@
         <v>7</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>1</v>
@@ -1239,16 +1239,16 @@
         <v>1</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="S11" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="U11" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="V11" s="1" t="s">
         <v>5</v>
@@ -1262,13 +1262,13 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>7</v>
@@ -1277,10 +1277,10 @@
         <v>7</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>1</v>
@@ -1313,13 +1313,13 @@
         <v>1</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="S12" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="T12" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="U12" s="1" t="s">
         <v>5</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>7</v>
@@ -1351,10 +1351,10 @@
         <v>7</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>1</v>
@@ -1387,10 +1387,10 @@
         <v>1</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="S13" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="T13" s="1" t="s">
         <v>5</v>
@@ -1410,25 +1410,25 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>1</v>
@@ -1461,7 +1461,7 @@
         <v>1</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="S14" s="1" t="s">
         <v>5</v>
@@ -1470,10 +1470,10 @@
         <v>5</v>
       </c>
       <c r="U14" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="V14" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="W14" s="1" t="s">
         <v>5</v>
@@ -1484,73 +1484,73 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="T15" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="U15" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="V15" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="W15" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="X15">
         <v>14</v>
@@ -1558,73 +1558,73 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="R16" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="T16" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="U16" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="V16" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="W16" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="X16">
         <v>15</v>
@@ -1632,73 +1632,73 @@
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="R17" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="S17" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="T17" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="U17" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="V17" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="W17" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="X17">
         <v>16</v>
@@ -1706,28 +1706,28 @@
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>6</v>
@@ -1739,7 +1739,7 @@
         <v>6</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>6</v>
@@ -1751,25 +1751,25 @@
         <v>6</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="S18" s="1" t="s">
         <v>3</v>
       </c>
       <c r="T18" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U18" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="V18" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W18" s="1" t="s">
         <v>3</v>
@@ -1795,13 +1795,13 @@
         <v>8</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>6</v>
@@ -1825,13 +1825,13 @@
         <v>6</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="R19" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="S19" s="1" t="s">
         <v>3</v>
@@ -1866,20 +1866,20 @@
         <v>8</v>
       </c>
       <c r="E20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="J20" s="1" t="s">
         <v>6</v>
       </c>
@@ -1896,16 +1896,16 @@
         <v>6</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="S20" s="1" t="s">
         <v>3</v>
@@ -1940,16 +1940,16 @@
         <v>8</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>6</v>
@@ -1973,13 +1973,13 @@
         <v>6</v>
       </c>
       <c r="P21" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="Q21" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="R21" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="S21" s="1" t="s">
         <v>3</v>
@@ -2017,13 +2017,13 @@
         <v>8</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>6</v>
@@ -2047,13 +2047,13 @@
         <v>6</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="R22" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="S22" s="1" t="s">
         <v>3</v>
@@ -2091,13 +2091,13 @@
         <v>8</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>6</v>
@@ -2121,13 +2121,13 @@
         <v>6</v>
       </c>
       <c r="P23" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="R23" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="S23" s="1" t="s">
         <v>3</v>
@@ -2165,13 +2165,13 @@
         <v>8</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>6</v>
@@ -2195,13 +2195,13 @@
         <v>6</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="R24" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="S24" s="1" t="s">
         <v>3</v>
@@ -2239,13 +2239,13 @@
         <v>8</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>6</v>
@@ -2269,13 +2269,13 @@
         <v>6</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="Q25" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="R25" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="S25" s="1" t="s">
         <v>3</v>
@@ -2313,13 +2313,13 @@
         <v>8</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>6</v>
@@ -2343,13 +2343,13 @@
         <v>6</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="Q26" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="R26" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="S26" s="1" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
added CR_BoardAdjTargetTest.java and updated our Our_ClueLyout.xlsx.
</commit_message>
<xml_diff>
--- a/Our_ClueLayout.xlsx
+++ b/Our_ClueLayout.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="30">
   <si>
     <t>C</t>
   </si>
@@ -93,13 +93,34 @@
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>Number of doors: 17</t>
+  </si>
+  <si>
+    <t>White: Door direction tests</t>
+  </si>
+  <si>
+    <t>Orange: adjacency list tests, inside room</t>
+  </si>
+  <si>
+    <t>Purple: adjancecy list tests, room exits</t>
+  </si>
+  <si>
+    <t>Green: adjacency lists beside room entrace</t>
+  </si>
+  <si>
+    <t>Brown: walkway scenarios</t>
+  </si>
+  <si>
+    <t>Pink: test targets</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,8 +128,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,6 +166,42 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -152,18 +215,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF00FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -438,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X27"/>
+  <dimension ref="A1:X36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +531,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="11" t="s">
         <v>22</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -521,7 +596,7 @@
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -584,7 +659,7 @@
       <c r="U2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="V2" s="7" t="s">
         <v>4</v>
       </c>
       <c r="W2" s="1" t="s">
@@ -607,10 +682,10 @@
       <c r="D3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="E3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -631,7 +706,7 @@
       <c r="L3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="7" t="s">
         <v>9</v>
       </c>
       <c r="N3" s="1" t="s">
@@ -693,7 +768,7 @@
       <c r="H4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="8" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="4" t="s">
@@ -746,7 +821,7 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -788,7 +863,7 @@
       <c r="O5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="P5" s="6" t="s">
         <v>13</v>
       </c>
       <c r="Q5" s="3" t="s">
@@ -803,7 +878,7 @@
       <c r="T5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="U5" s="4" t="s">
+      <c r="U5" s="6" t="s">
         <v>14</v>
       </c>
       <c r="V5" s="4" t="s">
@@ -880,7 +955,7 @@
       <c r="U6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="V6" s="3" t="s">
+      <c r="V6" s="10" t="s">
         <v>22</v>
       </c>
       <c r="W6" s="3" t="s">
@@ -891,7 +966,7 @@
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -927,7 +1002,7 @@
       <c r="L7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="M7" s="11" t="s">
         <v>22</v>
       </c>
       <c r="N7" s="3" t="s">
@@ -1190,7 +1265,7 @@
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1267,7 +1342,7 @@
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="11" t="s">
         <v>22</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1318,7 +1393,7 @@
       <c r="S12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="T12" s="3" t="s">
+      <c r="T12" s="8" t="s">
         <v>22</v>
       </c>
       <c r="U12" s="1" t="s">
@@ -1516,7 +1591,7 @@
       <c r="K15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="L15" s="8" t="s">
         <v>22</v>
       </c>
       <c r="M15" s="3" t="s">
@@ -1575,7 +1650,7 @@
       <c r="F16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H16" s="3" t="s">
@@ -1691,7 +1766,7 @@
       <c r="T17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="U17" s="3" t="s">
+      <c r="U17" s="10" t="s">
         <v>22</v>
       </c>
       <c r="V17" s="3" t="s">
@@ -1705,7 +1780,7 @@
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -1738,7 +1813,7 @@
       <c r="K18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L18" s="4" t="s">
+      <c r="L18" s="6" t="s">
         <v>20</v>
       </c>
       <c r="M18" s="1" t="s">
@@ -1762,7 +1837,7 @@
       <c r="S18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="T18" s="4" t="s">
+      <c r="T18" s="9" t="s">
         <v>16</v>
       </c>
       <c r="U18" s="4" t="s">
@@ -1865,7 +1940,7 @@
       <c r="D20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="9" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="3" t="s">
@@ -1877,7 +1952,7 @@
       <c r="H20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="I20" s="9" t="s">
         <v>19</v>
       </c>
       <c r="J20" s="1" t="s">
@@ -1898,7 +1973,7 @@
       <c r="O20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="P20" s="3" t="s">
+      <c r="P20" s="10" t="s">
         <v>22</v>
       </c>
       <c r="Q20" s="3" t="s">
@@ -2016,7 +2091,7 @@
       <c r="E22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="11" t="s">
         <v>22</v>
       </c>
       <c r="G22" s="3" t="s">
@@ -2105,7 +2180,7 @@
       <c r="J23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="K23" s="7" t="s">
         <v>6</v>
       </c>
       <c r="L23" s="1" t="s">
@@ -2123,7 +2198,7 @@
       <c r="P23" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Q23" s="3" t="s">
+      <c r="Q23" s="8" t="s">
         <v>22</v>
       </c>
       <c r="R23" s="3" t="s">
@@ -2262,7 +2337,7 @@
       <c r="M25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N25" s="1" t="s">
+      <c r="N25" s="7" t="s">
         <v>6</v>
       </c>
       <c r="O25" s="1" t="s">
@@ -2297,7 +2372,7 @@
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -2312,7 +2387,7 @@
       <c r="E26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="6" t="s">
         <v>22</v>
       </c>
       <c r="G26" s="3" t="s">
@@ -2440,6 +2515,46 @@
       <c r="W27">
         <v>22</v>
       </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="6"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="J34" s="6"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>29</v>
+      </c>
+      <c r="H36" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finished up making failing tests for adjacency and target testing.
</commit_message>
<xml_diff>
--- a/Our_ClueLayout.xlsx
+++ b/Our_ClueLayout.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\workspace\ClueGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24960" windowHeight="8070"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -516,7 +516,7 @@
   <dimension ref="A1:X36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1313,7 +1313,7 @@
       <c r="Q11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="R11" s="3" t="s">
+      <c r="R11" s="11" t="s">
         <v>22</v>
       </c>
       <c r="S11" s="3" t="s">

</xml_diff>

<commit_message>
gui for display board and detective notes done.
</commit_message>
<xml_diff>
--- a/Our_ClueLayout.xlsx
+++ b/Our_ClueLayout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\ClueGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\workspace\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -516,7 +516,7 @@
   <dimension ref="A1:X36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>